<commit_message>
Update Evaluation Grid / CeTi ONIP
</commit_message>
<xml_diff>
--- a/_autres/Grilles_Eval.xlsx
+++ b/_autres/Grilles_Eval.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tools\git_repo\digital_methods\semester-5\ONIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tools\git_repo\digital_methods\semester-5\_autres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DA18A7-8336-4759-A2E0-6FCC34C50446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FD259F-46F3-42AC-8E34-43D4B374C4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="v2" sheetId="2" r:id="rId1"/>
+    <sheet name="ONIP" sheetId="2" r:id="rId1"/>
+    <sheet name="CeTI" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="43">
   <si>
     <t xml:space="preserve">NOMS : </t>
   </si>
@@ -106,6 +107,54 @@
   </si>
   <si>
     <t>Analyse des données et validation modèle</t>
+  </si>
+  <si>
+    <t>INSTRUMENTATION</t>
+  </si>
+  <si>
+    <t>Paramètrage des instruments</t>
+  </si>
+  <si>
+    <t>Instruments de mesure pertinents / Cablage</t>
+  </si>
+  <si>
+    <t>Dipôle</t>
+  </si>
+  <si>
+    <t>Système</t>
+  </si>
+  <si>
+    <t>PROTOCOLE SPECIFIQUE</t>
+  </si>
+  <si>
+    <t>Résultats pertinents basés sur données exp.</t>
+  </si>
+  <si>
+    <t>Génération de signaux pertinentes de tests</t>
+  </si>
+  <si>
+    <t>Validation fonctionnement linéaire</t>
+  </si>
+  <si>
+    <t>Comportement global</t>
+  </si>
+  <si>
+    <t>Gain du système</t>
+  </si>
+  <si>
+    <t>Bande-passante du système</t>
+  </si>
+  <si>
+    <t>Ordre du système</t>
+  </si>
+  <si>
+    <t>CeTI-TP / Conception Electronique - TP</t>
+  </si>
+  <si>
+    <t>Evaluation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOM : </t>
   </si>
 </sst>
 </file>
@@ -222,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -252,6 +301,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -273,12 +328,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,8 +622,8 @@
   </sheetPr>
   <dimension ref="A1:AN33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM11" sqref="AM11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,46 +642,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="T1" s="20" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="T1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
     </row>
     <row r="3" spans="1:40" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
@@ -675,18 +733,18 @@
       <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="23"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="25"/>
       <c r="T4" s="2" t="s">
         <v>1</v>
       </c>
@@ -694,18 +752,18 @@
       <c r="V4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="23"/>
-      <c r="AC4" s="21"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="23"/>
-      <c r="AH4" s="21"/>
-      <c r="AI4" s="22"/>
-      <c r="AJ4" s="22"/>
-      <c r="AK4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="25"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="25"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="24"/>
+      <c r="AJ4" s="24"/>
+      <c r="AK4" s="25"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="E5" s="7"/>
@@ -734,42 +792,42 @@
       <c r="AK5" s="7"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-      <c r="J6" s="17" t="s">
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+      <c r="J6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="19"/>
-      <c r="O6" s="17" t="s">
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="21"/>
+      <c r="O6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="19"/>
-      <c r="X6" s="17" t="s">
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="21"/>
+      <c r="X6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="19"/>
-      <c r="AC6" s="17" t="s">
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="21"/>
+      <c r="AC6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="18"/>
-      <c r="AE6" s="18"/>
-      <c r="AF6" s="19"/>
-      <c r="AH6" s="17" t="s">
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="21"/>
+      <c r="AH6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AI6" s="18"/>
-      <c r="AJ6" s="18"/>
-      <c r="AK6" s="19"/>
+      <c r="AI6" s="20"/>
+      <c r="AJ6" s="20"/>
+      <c r="AK6" s="21"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
@@ -903,7 +961,7 @@
       <c r="AI8" s="16"/>
       <c r="AJ8" s="16"/>
       <c r="AK8" s="16"/>
-      <c r="AN8" s="25"/>
+      <c r="AN8" s="18"/>
     </row>
     <row r="9" spans="1:40" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
@@ -942,7 +1000,7 @@
       <c r="AI9" s="12"/>
       <c r="AJ9" s="12"/>
       <c r="AK9" s="12"/>
-      <c r="AN9" s="25"/>
+      <c r="AN9" s="18"/>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
@@ -985,7 +1043,7 @@
       <c r="AI10" s="16"/>
       <c r="AJ10" s="16"/>
       <c r="AK10" s="16"/>
-      <c r="AN10" s="25"/>
+      <c r="AN10" s="18"/>
     </row>
     <row r="11" spans="1:40" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
@@ -1024,7 +1082,7 @@
       <c r="AI11" s="12"/>
       <c r="AJ11" s="12"/>
       <c r="AK11" s="12"/>
-      <c r="AN11" s="25"/>
+      <c r="AN11" s="18"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
@@ -1067,7 +1125,7 @@
       <c r="AI12" s="16"/>
       <c r="AJ12" s="16"/>
       <c r="AK12" s="16"/>
-      <c r="AN12" s="25"/>
+      <c r="AN12" s="18"/>
     </row>
     <row r="13" spans="1:40" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
@@ -1106,7 +1164,7 @@
       <c r="AI13" s="12"/>
       <c r="AJ13" s="12"/>
       <c r="AK13" s="12"/>
-      <c r="AN13" s="25"/>
+      <c r="AN13" s="18"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
@@ -1149,9 +1207,9 @@
       <c r="AI14" s="16"/>
       <c r="AJ14" s="16"/>
       <c r="AK14" s="16"/>
-      <c r="AN14" s="25"/>
-    </row>
-    <row r="15" spans="1:40" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AN14" s="18"/>
+    </row>
+    <row r="15" spans="1:40" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="U15" s="10"/>
@@ -1274,7 +1332,7 @@
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
-      <c r="AN17" s="25"/>
+      <c r="AN17" s="18"/>
     </row>
     <row r="18" spans="1:40" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10"/>
@@ -1315,7 +1373,7 @@
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
-      <c r="AN19" s="25"/>
+      <c r="AN19" s="18"/>
     </row>
     <row r="20" spans="1:40" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="10"/>
@@ -1356,7 +1414,7 @@
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
-      <c r="AN21" s="25"/>
+      <c r="AN21" s="18"/>
     </row>
     <row r="22" spans="1:40" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
@@ -1397,14 +1455,14 @@
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
-      <c r="AN23" s="25"/>
+      <c r="AN23" s="18"/>
     </row>
     <row r="24" spans="1:40" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
-      <c r="AN24" s="25"/>
+      <c r="AN24" s="18"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
@@ -1439,14 +1497,14 @@
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
-      <c r="AN25" s="25"/>
-    </row>
-    <row r="26" spans="1:40" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AN25" s="18"/>
+    </row>
+    <row r="26" spans="1:40" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
-      <c r="AN26" s="25"/>
+      <c r="AN26" s="18"/>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
@@ -1537,7 +1595,7 @@
       <c r="AK27" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AN27" s="25"/>
+      <c r="AN27" s="18"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
@@ -1580,7 +1638,7 @@
       <c r="AI28" s="16"/>
       <c r="AJ28" s="16"/>
       <c r="AK28" s="16"/>
-      <c r="AN28" s="25"/>
+      <c r="AN28" s="18"/>
     </row>
     <row r="29" spans="1:40" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
@@ -1661,7 +1719,7 @@
       <c r="AI30" s="16"/>
       <c r="AJ30" s="16"/>
       <c r="AK30" s="16"/>
-      <c r="AN30" s="25"/>
+      <c r="AN30" s="18"/>
     </row>
     <row r="31" spans="1:40" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
@@ -1700,7 +1758,7 @@
       <c r="AI31" s="12"/>
       <c r="AJ31" s="12"/>
       <c r="AK31" s="12"/>
-      <c r="AN31" s="24"/>
+      <c r="AN31" s="17"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
@@ -1743,7 +1801,7 @@
       <c r="AI32" s="16"/>
       <c r="AJ32" s="16"/>
       <c r="AK32" s="16"/>
-      <c r="AN32" s="25"/>
+      <c r="AN32" s="18"/>
     </row>
     <row r="33" spans="2:22" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="10"/>
@@ -1771,4 +1829,833 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="88" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B644CA8-83FA-497A-BA3A-AEE92BB48830}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AA29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="1.6640625" customWidth="1"/>
+    <col min="5" max="8" width="2.77734375" customWidth="1"/>
+    <col min="9" max="9" width="1.6640625" customWidth="1"/>
+    <col min="10" max="13" width="2.77734375" customWidth="1"/>
+    <col min="14" max="14" width="4.77734375" customWidth="1"/>
+    <col min="15" max="15" width="5" customWidth="1"/>
+    <col min="16" max="16" width="17.5546875" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" customWidth="1"/>
+    <col min="18" max="18" width="1.6640625" customWidth="1"/>
+    <col min="19" max="22" width="2.77734375" customWidth="1"/>
+    <col min="23" max="23" width="1.6640625" customWidth="1"/>
+    <col min="24" max="27" width="2.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+    </row>
+    <row r="3" spans="1:27" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25"/>
+      <c r="O4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="23"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="25"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="25"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="E5" s="7"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="7"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="E6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+      <c r="J6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="21"/>
+      <c r="S6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="21"/>
+      <c r="X6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="21"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="T7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="V7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="W7" s="12"/>
+      <c r="X7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA7" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="12"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="16"/>
+    </row>
+    <row r="9" spans="1:27" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="12"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="12"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="16"/>
+    </row>
+    <row r="11" spans="1:27" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="R12" s="12"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="16"/>
+    </row>
+    <row r="13" spans="1:27" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="27"/>
+      <c r="J14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="27"/>
+      <c r="X14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA14" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+    </row>
+    <row r="18" spans="1:27" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+    </row>
+    <row r="20" spans="1:27" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
+      <c r="V21" s="29"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+    </row>
+    <row r="22" spans="1:27" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="12"/>
+      <c r="J23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="O23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="T23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="U23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="V23" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="W23" s="12"/>
+      <c r="X23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA23" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="R24" s="12"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="16"/>
+      <c r="Y24" s="16"/>
+      <c r="Z24" s="16"/>
+      <c r="AA24" s="16"/>
+    </row>
+    <row r="25" spans="1:27" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12"/>
+      <c r="AA25" s="12"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A26" s="12"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="R26" s="12"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="16"/>
+    </row>
+    <row r="27" spans="1:27" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="12"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="R28" s="12"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="16"/>
+      <c r="Y28" s="16"/>
+      <c r="Z28" s="16"/>
+      <c r="AA28" s="16"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="X6:AA6"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="O1:AA1"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="X4:AA4"/>
+    <mergeCell ref="S6:V6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="99" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Eval Grid ONIP
</commit_message>
<xml_diff>
--- a/_autres/Grilles_Eval.xlsx
+++ b/_autres/Grilles_Eval.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\git_repo\digital_methods\semester-5\_autres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70039F1D-47F0-42FC-B0B3-45009817671C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DADA771-953B-42DF-B88B-656E2D0DC0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ONIP" sheetId="2" r:id="rId1"/>
-    <sheet name="CeTI" sheetId="3" r:id="rId2"/>
-    <sheet name="CeTI_prof" sheetId="4" r:id="rId3"/>
+    <sheet name="ONIP_prof" sheetId="5" r:id="rId2"/>
+    <sheet name="CeTI" sheetId="3" r:id="rId3"/>
+    <sheet name="CeTI_prof" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="45">
   <si>
     <t xml:space="preserve">NOMS : </t>
   </si>
@@ -157,6 +158,12 @@
   <si>
     <t>Date</t>
   </si>
+  <si>
+    <t xml:space="preserve">Date : </t>
+  </si>
+  <si>
+    <t>ONIP / Evaluation / BLOC ____</t>
+  </si>
 </sst>
 </file>
 
@@ -243,7 +250,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -340,11 +347,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -399,6 +486,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,6 +510,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,9 +555,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,46 +860,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="T1" s="33" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="T1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
     </row>
     <row r="3" spans="1:40" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
@@ -837,18 +951,18 @@
       <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="36"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="36"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="36"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="39"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="39"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="39"/>
       <c r="T4" s="2" t="s">
         <v>1</v>
       </c>
@@ -856,18 +970,18 @@
       <c r="V4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="36"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="36"/>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="35"/>
-      <c r="AJ4" s="35"/>
-      <c r="AK4" s="36"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="39"/>
+      <c r="AC4" s="37"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="39"/>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="38"/>
+      <c r="AJ4" s="38"/>
+      <c r="AK4" s="39"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="E5" s="7"/>
@@ -896,42 +1010,42 @@
       <c r="AK5" s="7"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-      <c r="J6" s="30" t="s">
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="35"/>
+      <c r="J6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="32"/>
-      <c r="O6" s="30" t="s">
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="35"/>
+      <c r="O6" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="32"/>
-      <c r="X6" s="30" t="s">
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="35"/>
+      <c r="X6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" s="31"/>
-      <c r="Z6" s="31"/>
-      <c r="AA6" s="32"/>
-      <c r="AC6" s="30" t="s">
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="34"/>
+      <c r="AA6" s="35"/>
+      <c r="AC6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="31"/>
-      <c r="AE6" s="31"/>
-      <c r="AF6" s="32"/>
-      <c r="AH6" s="30" t="s">
+      <c r="AD6" s="34"/>
+      <c r="AE6" s="34"/>
+      <c r="AF6" s="35"/>
+      <c r="AH6" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="AI6" s="31"/>
-      <c r="AJ6" s="31"/>
-      <c r="AK6" s="32"/>
+      <c r="AI6" s="34"/>
+      <c r="AJ6" s="34"/>
+      <c r="AK6" s="35"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -1936,6 +2050,2490 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC324C7E-ACD4-4C9D-979D-35F7BD0500EB}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AQ63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="10" max="13" width="4.7109375" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" customWidth="1"/>
+    <col min="15" max="18" width="4.7109375" customWidth="1"/>
+    <col min="19" max="19" width="2.7109375" customWidth="1"/>
+    <col min="20" max="23" width="4.7109375" customWidth="1"/>
+    <col min="24" max="24" width="2.7109375" customWidth="1"/>
+    <col min="25" max="28" width="4.7109375" customWidth="1"/>
+    <col min="29" max="29" width="2.7109375" customWidth="1"/>
+    <col min="30" max="33" width="4.7109375" customWidth="1"/>
+    <col min="34" max="34" width="2.7109375" customWidth="1"/>
+    <col min="35" max="38" width="4.7109375" customWidth="1"/>
+    <col min="39" max="39" width="2.7109375" customWidth="1"/>
+    <col min="40" max="43" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="10"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="42"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="42"/>
+      <c r="Y3" s="40"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="42"/>
+      <c r="AD3" s="40"/>
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="41"/>
+      <c r="AG3" s="42"/>
+      <c r="AI3" s="40"/>
+      <c r="AJ3" s="41"/>
+      <c r="AK3" s="41"/>
+      <c r="AL3" s="42"/>
+      <c r="AN3" s="40"/>
+      <c r="AO3" s="41"/>
+      <c r="AP3" s="41"/>
+      <c r="AQ3" s="42"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="45"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="45"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="45"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="45"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="44"/>
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="45"/>
+      <c r="AD4" s="43"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
+      <c r="AG4" s="45"/>
+      <c r="AI4" s="43"/>
+      <c r="AJ4" s="44"/>
+      <c r="AK4" s="44"/>
+      <c r="AL4" s="45"/>
+      <c r="AN4" s="43"/>
+      <c r="AO4" s="44"/>
+      <c r="AP4" s="44"/>
+      <c r="AQ4" s="45"/>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="E5" s="46"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="48"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="48"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="48"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="47"/>
+      <c r="W5" s="48"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="48"/>
+      <c r="AD5" s="46"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="48"/>
+      <c r="AI5" s="46"/>
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="47"/>
+      <c r="AL5" s="48"/>
+      <c r="AN5" s="46"/>
+      <c r="AO5" s="47"/>
+      <c r="AP5" s="47"/>
+      <c r="AQ5" s="48"/>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="12"/>
+      <c r="O6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" s="12"/>
+      <c r="T6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="U6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="V6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="W6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH6" s="12"/>
+      <c r="AI6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM6" s="12"/>
+      <c r="AN6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ6" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="16"/>
+      <c r="AH7" s="12"/>
+      <c r="AI7" s="16"/>
+      <c r="AJ7" s="16"/>
+      <c r="AK7" s="16"/>
+      <c r="AL7" s="16"/>
+      <c r="AM7" s="12"/>
+      <c r="AN7" s="16"/>
+      <c r="AO7" s="16"/>
+      <c r="AP7" s="16"/>
+      <c r="AQ7" s="16"/>
+    </row>
+    <row r="8" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="12"/>
+      <c r="AF8" s="12"/>
+      <c r="AG8" s="12"/>
+      <c r="AH8" s="12"/>
+      <c r="AI8" s="12"/>
+      <c r="AJ8" s="12"/>
+      <c r="AK8" s="12"/>
+      <c r="AL8" s="12"/>
+      <c r="AM8" s="12"/>
+      <c r="AN8" s="12"/>
+      <c r="AO8" s="12"/>
+      <c r="AP8" s="12"/>
+      <c r="AQ8" s="12"/>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="12"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9" s="16"/>
+      <c r="AF9" s="16"/>
+      <c r="AG9" s="16"/>
+      <c r="AH9" s="12"/>
+      <c r="AI9" s="16"/>
+      <c r="AJ9" s="16"/>
+      <c r="AK9" s="16"/>
+      <c r="AL9" s="16"/>
+      <c r="AM9" s="12"/>
+      <c r="AN9" s="16"/>
+      <c r="AO9" s="16"/>
+      <c r="AP9" s="16"/>
+      <c r="AQ9" s="16"/>
+    </row>
+    <row r="10" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12"/>
+      <c r="AH10" s="12"/>
+      <c r="AI10" s="12"/>
+      <c r="AJ10" s="12"/>
+      <c r="AK10" s="12"/>
+      <c r="AL10" s="12"/>
+      <c r="AM10" s="12"/>
+      <c r="AN10" s="12"/>
+      <c r="AO10" s="12"/>
+      <c r="AP10" s="12"/>
+      <c r="AQ10" s="12"/>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="16"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="16"/>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="16"/>
+      <c r="AH11" s="12"/>
+      <c r="AI11" s="16"/>
+      <c r="AJ11" s="16"/>
+      <c r="AK11" s="16"/>
+      <c r="AL11" s="16"/>
+      <c r="AM11" s="12"/>
+      <c r="AN11" s="16"/>
+      <c r="AO11" s="16"/>
+      <c r="AP11" s="16"/>
+      <c r="AQ11" s="16"/>
+    </row>
+    <row r="12" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="12"/>
+      <c r="AD12" s="12"/>
+      <c r="AE12" s="12"/>
+      <c r="AF12" s="12"/>
+      <c r="AG12" s="12"/>
+      <c r="AH12" s="12"/>
+      <c r="AI12" s="12"/>
+      <c r="AJ12" s="12"/>
+      <c r="AK12" s="12"/>
+      <c r="AL12" s="12"/>
+      <c r="AM12" s="12"/>
+      <c r="AN12" s="12"/>
+      <c r="AO12" s="12"/>
+      <c r="AP12" s="12"/>
+      <c r="AQ12" s="12"/>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="16"/>
+      <c r="Z13" s="16"/>
+      <c r="AA13" s="16"/>
+      <c r="AB13" s="16"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="16"/>
+      <c r="AE13" s="16"/>
+      <c r="AF13" s="16"/>
+      <c r="AG13" s="16"/>
+      <c r="AH13" s="12"/>
+      <c r="AI13" s="16"/>
+      <c r="AJ13" s="16"/>
+      <c r="AK13" s="16"/>
+      <c r="AL13" s="16"/>
+      <c r="AM13" s="12"/>
+      <c r="AN13" s="16"/>
+      <c r="AO13" s="16"/>
+      <c r="AP13" s="16"/>
+      <c r="AQ13" s="16"/>
+    </row>
+    <row r="14" spans="1:43" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="E15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="U15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ15" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+    </row>
+    <row r="17" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AN18" s="1"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
+    </row>
+    <row r="19" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="1"/>
+      <c r="AK20" s="1"/>
+      <c r="AL20" s="1"/>
+      <c r="AN20" s="1"/>
+      <c r="AO20" s="1"/>
+      <c r="AP20" s="1"/>
+      <c r="AQ20" s="1"/>
+    </row>
+    <row r="21" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="1"/>
+      <c r="AL22" s="1"/>
+      <c r="AN22" s="1"/>
+      <c r="AO22" s="1"/>
+      <c r="AP22" s="1"/>
+      <c r="AQ22" s="1"/>
+    </row>
+    <row r="23" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+      <c r="AI24" s="1"/>
+      <c r="AJ24" s="1"/>
+      <c r="AK24" s="1"/>
+      <c r="AL24" s="1"/>
+      <c r="AN24" s="1"/>
+      <c r="AO24" s="1"/>
+      <c r="AP24" s="1"/>
+      <c r="AQ24" s="1"/>
+    </row>
+    <row r="25" spans="1:43" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="12"/>
+      <c r="J26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="N26" s="12"/>
+      <c r="O26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="P26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="R26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S26" s="12"/>
+      <c r="T26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="U26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="V26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="W26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH26" s="12"/>
+      <c r="AI26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM26" s="12"/>
+      <c r="AN26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ26" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="16"/>
+      <c r="Z27" s="16"/>
+      <c r="AA27" s="16"/>
+      <c r="AB27" s="16"/>
+      <c r="AC27" s="12"/>
+      <c r="AD27" s="16"/>
+      <c r="AE27" s="16"/>
+      <c r="AF27" s="16"/>
+      <c r="AG27" s="16"/>
+      <c r="AH27" s="12"/>
+      <c r="AI27" s="16"/>
+      <c r="AJ27" s="16"/>
+      <c r="AK27" s="16"/>
+      <c r="AL27" s="16"/>
+      <c r="AM27" s="12"/>
+      <c r="AN27" s="16"/>
+      <c r="AO27" s="16"/>
+      <c r="AP27" s="16"/>
+      <c r="AQ27" s="16"/>
+    </row>
+    <row r="28" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12"/>
+      <c r="AD28" s="12"/>
+      <c r="AE28" s="12"/>
+      <c r="AF28" s="12"/>
+      <c r="AG28" s="12"/>
+      <c r="AH28" s="12"/>
+      <c r="AI28" s="12"/>
+      <c r="AJ28" s="12"/>
+      <c r="AK28" s="12"/>
+      <c r="AL28" s="12"/>
+      <c r="AM28" s="12"/>
+      <c r="AN28" s="12"/>
+      <c r="AO28" s="12"/>
+      <c r="AP28" s="12"/>
+      <c r="AQ28" s="12"/>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="16"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="12"/>
+      <c r="Y29" s="16"/>
+      <c r="Z29" s="16"/>
+      <c r="AA29" s="16"/>
+      <c r="AB29" s="16"/>
+      <c r="AC29" s="12"/>
+      <c r="AD29" s="16"/>
+      <c r="AE29" s="16"/>
+      <c r="AF29" s="16"/>
+      <c r="AG29" s="16"/>
+      <c r="AH29" s="12"/>
+      <c r="AI29" s="16"/>
+      <c r="AJ29" s="16"/>
+      <c r="AK29" s="16"/>
+      <c r="AL29" s="16"/>
+      <c r="AM29" s="12"/>
+      <c r="AN29" s="16"/>
+      <c r="AO29" s="16"/>
+      <c r="AP29" s="16"/>
+      <c r="AQ29" s="16"/>
+    </row>
+    <row r="30" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
+      <c r="AA30" s="12"/>
+      <c r="AB30" s="12"/>
+      <c r="AC30" s="12"/>
+      <c r="AD30" s="12"/>
+      <c r="AE30" s="12"/>
+      <c r="AF30" s="12"/>
+      <c r="AG30" s="12"/>
+      <c r="AH30" s="12"/>
+      <c r="AI30" s="12"/>
+      <c r="AJ30" s="12"/>
+      <c r="AK30" s="12"/>
+      <c r="AL30" s="12"/>
+      <c r="AM30" s="12"/>
+      <c r="AN30" s="12"/>
+      <c r="AO30" s="12"/>
+      <c r="AP30" s="12"/>
+      <c r="AQ30" s="12"/>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="16"/>
+      <c r="X31" s="12"/>
+      <c r="Y31" s="16"/>
+      <c r="Z31" s="16"/>
+      <c r="AA31" s="16"/>
+      <c r="AB31" s="16"/>
+      <c r="AC31" s="12"/>
+      <c r="AD31" s="16"/>
+      <c r="AE31" s="16"/>
+      <c r="AF31" s="16"/>
+      <c r="AG31" s="16"/>
+      <c r="AH31" s="12"/>
+      <c r="AI31" s="16"/>
+      <c r="AJ31" s="16"/>
+      <c r="AK31" s="16"/>
+      <c r="AL31" s="16"/>
+      <c r="AM31" s="12"/>
+      <c r="AN31" s="16"/>
+      <c r="AO31" s="16"/>
+      <c r="AP31" s="16"/>
+      <c r="AQ31" s="16"/>
+    </row>
+    <row r="32" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="10"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="42"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="41"/>
+      <c r="M35" s="42"/>
+      <c r="O35" s="40"/>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="41"/>
+      <c r="R35" s="42"/>
+      <c r="T35" s="40"/>
+      <c r="U35" s="41"/>
+      <c r="V35" s="41"/>
+      <c r="W35" s="42"/>
+      <c r="Y35" s="40"/>
+      <c r="Z35" s="41"/>
+      <c r="AA35" s="41"/>
+      <c r="AB35" s="42"/>
+      <c r="AD35" s="40"/>
+      <c r="AE35" s="41"/>
+      <c r="AF35" s="41"/>
+      <c r="AG35" s="42"/>
+      <c r="AI35" s="40"/>
+      <c r="AJ35" s="41"/>
+      <c r="AK35" s="41"/>
+      <c r="AL35" s="42"/>
+      <c r="AN35" s="40"/>
+      <c r="AO35" s="41"/>
+      <c r="AP35" s="41"/>
+      <c r="AQ35" s="42"/>
+    </row>
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="45"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="45"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="44"/>
+      <c r="Q36" s="44"/>
+      <c r="R36" s="45"/>
+      <c r="T36" s="43"/>
+      <c r="U36" s="44"/>
+      <c r="V36" s="44"/>
+      <c r="W36" s="45"/>
+      <c r="Y36" s="43"/>
+      <c r="Z36" s="44"/>
+      <c r="AA36" s="44"/>
+      <c r="AB36" s="45"/>
+      <c r="AD36" s="43"/>
+      <c r="AE36" s="44"/>
+      <c r="AF36" s="44"/>
+      <c r="AG36" s="45"/>
+      <c r="AI36" s="43"/>
+      <c r="AJ36" s="44"/>
+      <c r="AK36" s="44"/>
+      <c r="AL36" s="45"/>
+      <c r="AN36" s="43"/>
+      <c r="AO36" s="44"/>
+      <c r="AP36" s="44"/>
+      <c r="AQ36" s="45"/>
+    </row>
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="E37" s="46"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="48"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="47"/>
+      <c r="L37" s="47"/>
+      <c r="M37" s="48"/>
+      <c r="O37" s="46"/>
+      <c r="P37" s="47"/>
+      <c r="Q37" s="47"/>
+      <c r="R37" s="48"/>
+      <c r="T37" s="46"/>
+      <c r="U37" s="47"/>
+      <c r="V37" s="47"/>
+      <c r="W37" s="48"/>
+      <c r="Y37" s="46"/>
+      <c r="Z37" s="47"/>
+      <c r="AA37" s="47"/>
+      <c r="AB37" s="48"/>
+      <c r="AD37" s="46"/>
+      <c r="AE37" s="47"/>
+      <c r="AF37" s="47"/>
+      <c r="AG37" s="48"/>
+      <c r="AI37" s="46"/>
+      <c r="AJ37" s="47"/>
+      <c r="AK37" s="47"/>
+      <c r="AL37" s="48"/>
+      <c r="AN37" s="46"/>
+      <c r="AO37" s="47"/>
+      <c r="AP37" s="47"/>
+      <c r="AQ37" s="48"/>
+    </row>
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="12"/>
+      <c r="J38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M38" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="N38" s="12"/>
+      <c r="O38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="P38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="R38" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S38" s="12"/>
+      <c r="T38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="U38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="V38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="W38" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="X38" s="12"/>
+      <c r="Y38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB38" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC38" s="12"/>
+      <c r="AD38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG38" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH38" s="12"/>
+      <c r="AI38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL38" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM38" s="12"/>
+      <c r="AN38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ38" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="12"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="12"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
+      <c r="V39" s="16"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="12"/>
+      <c r="Y39" s="16"/>
+      <c r="Z39" s="16"/>
+      <c r="AA39" s="16"/>
+      <c r="AB39" s="16"/>
+      <c r="AC39" s="12"/>
+      <c r="AD39" s="16"/>
+      <c r="AE39" s="16"/>
+      <c r="AF39" s="16"/>
+      <c r="AG39" s="16"/>
+      <c r="AH39" s="12"/>
+      <c r="AI39" s="16"/>
+      <c r="AJ39" s="16"/>
+      <c r="AK39" s="16"/>
+      <c r="AL39" s="16"/>
+      <c r="AM39" s="12"/>
+      <c r="AN39" s="16"/>
+      <c r="AO39" s="16"/>
+      <c r="AP39" s="16"/>
+      <c r="AQ39" s="16"/>
+    </row>
+    <row r="40" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="12"/>
+      <c r="S40" s="12"/>
+      <c r="T40" s="12"/>
+      <c r="U40" s="12"/>
+      <c r="V40" s="12"/>
+      <c r="W40" s="12"/>
+      <c r="X40" s="12"/>
+      <c r="Y40" s="12"/>
+      <c r="Z40" s="12"/>
+      <c r="AA40" s="12"/>
+      <c r="AB40" s="12"/>
+      <c r="AC40" s="12"/>
+      <c r="AD40" s="12"/>
+      <c r="AE40" s="12"/>
+      <c r="AF40" s="12"/>
+      <c r="AG40" s="12"/>
+      <c r="AH40" s="12"/>
+      <c r="AI40" s="12"/>
+      <c r="AJ40" s="12"/>
+      <c r="AK40" s="12"/>
+      <c r="AL40" s="12"/>
+      <c r="AM40" s="12"/>
+      <c r="AN40" s="12"/>
+      <c r="AO40" s="12"/>
+      <c r="AP40" s="12"/>
+      <c r="AQ40" s="12"/>
+    </row>
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="12"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="12"/>
+      <c r="T41" s="16"/>
+      <c r="U41" s="16"/>
+      <c r="V41" s="16"/>
+      <c r="W41" s="16"/>
+      <c r="X41" s="12"/>
+      <c r="Y41" s="16"/>
+      <c r="Z41" s="16"/>
+      <c r="AA41" s="16"/>
+      <c r="AB41" s="16"/>
+      <c r="AC41" s="12"/>
+      <c r="AD41" s="16"/>
+      <c r="AE41" s="16"/>
+      <c r="AF41" s="16"/>
+      <c r="AG41" s="16"/>
+      <c r="AH41" s="12"/>
+      <c r="AI41" s="16"/>
+      <c r="AJ41" s="16"/>
+      <c r="AK41" s="16"/>
+      <c r="AL41" s="16"/>
+      <c r="AM41" s="12"/>
+      <c r="AN41" s="16"/>
+      <c r="AO41" s="16"/>
+      <c r="AP41" s="16"/>
+      <c r="AQ41" s="16"/>
+    </row>
+    <row r="42" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+      <c r="P42" s="12"/>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12"/>
+      <c r="S42" s="12"/>
+      <c r="T42" s="12"/>
+      <c r="U42" s="12"/>
+      <c r="V42" s="12"/>
+      <c r="W42" s="12"/>
+      <c r="X42" s="12"/>
+      <c r="Y42" s="12"/>
+      <c r="Z42" s="12"/>
+      <c r="AA42" s="12"/>
+      <c r="AB42" s="12"/>
+      <c r="AC42" s="12"/>
+      <c r="AD42" s="12"/>
+      <c r="AE42" s="12"/>
+      <c r="AF42" s="12"/>
+      <c r="AG42" s="12"/>
+      <c r="AH42" s="12"/>
+      <c r="AI42" s="12"/>
+      <c r="AJ42" s="12"/>
+      <c r="AK42" s="12"/>
+      <c r="AL42" s="12"/>
+      <c r="AM42" s="12"/>
+      <c r="AN42" s="12"/>
+      <c r="AO42" s="12"/>
+      <c r="AP42" s="12"/>
+      <c r="AQ42" s="12"/>
+    </row>
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="12"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="12"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="16"/>
+      <c r="X43" s="12"/>
+      <c r="Y43" s="16"/>
+      <c r="Z43" s="16"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="16"/>
+      <c r="AC43" s="12"/>
+      <c r="AD43" s="16"/>
+      <c r="AE43" s="16"/>
+      <c r="AF43" s="16"/>
+      <c r="AG43" s="16"/>
+      <c r="AH43" s="12"/>
+      <c r="AI43" s="16"/>
+      <c r="AJ43" s="16"/>
+      <c r="AK43" s="16"/>
+      <c r="AL43" s="16"/>
+      <c r="AM43" s="12"/>
+      <c r="AN43" s="16"/>
+      <c r="AO43" s="16"/>
+      <c r="AP43" s="16"/>
+      <c r="AQ43" s="16"/>
+    </row>
+    <row r="44" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12"/>
+      <c r="S44" s="12"/>
+      <c r="T44" s="12"/>
+      <c r="U44" s="12"/>
+      <c r="V44" s="12"/>
+      <c r="W44" s="12"/>
+      <c r="X44" s="12"/>
+      <c r="Y44" s="12"/>
+      <c r="Z44" s="12"/>
+      <c r="AA44" s="12"/>
+      <c r="AB44" s="12"/>
+      <c r="AC44" s="12"/>
+      <c r="AD44" s="12"/>
+      <c r="AE44" s="12"/>
+      <c r="AF44" s="12"/>
+      <c r="AG44" s="12"/>
+      <c r="AH44" s="12"/>
+      <c r="AI44" s="12"/>
+      <c r="AJ44" s="12"/>
+      <c r="AK44" s="12"/>
+      <c r="AL44" s="12"/>
+      <c r="AM44" s="12"/>
+      <c r="AN44" s="12"/>
+      <c r="AO44" s="12"/>
+      <c r="AP44" s="12"/>
+      <c r="AQ44" s="12"/>
+    </row>
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="16"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="16"/>
+      <c r="U45" s="16"/>
+      <c r="V45" s="16"/>
+      <c r="W45" s="16"/>
+      <c r="X45" s="12"/>
+      <c r="Y45" s="16"/>
+      <c r="Z45" s="16"/>
+      <c r="AA45" s="16"/>
+      <c r="AB45" s="16"/>
+      <c r="AC45" s="12"/>
+      <c r="AD45" s="16"/>
+      <c r="AE45" s="16"/>
+      <c r="AF45" s="16"/>
+      <c r="AG45" s="16"/>
+      <c r="AH45" s="12"/>
+      <c r="AI45" s="16"/>
+      <c r="AJ45" s="16"/>
+      <c r="AK45" s="16"/>
+      <c r="AL45" s="16"/>
+      <c r="AM45" s="12"/>
+      <c r="AN45" s="16"/>
+      <c r="AO45" s="16"/>
+      <c r="AP45" s="16"/>
+      <c r="AQ45" s="16"/>
+    </row>
+    <row r="46" spans="1:43" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+    </row>
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="E47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="U47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="W47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ47" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B48" s="10"/>
+      <c r="C48" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="Y48" s="1"/>
+      <c r="Z48" s="1"/>
+      <c r="AA48" s="1"/>
+      <c r="AB48" s="1"/>
+      <c r="AD48" s="1"/>
+      <c r="AE48" s="1"/>
+      <c r="AF48" s="1"/>
+      <c r="AG48" s="1"/>
+      <c r="AI48" s="1"/>
+      <c r="AJ48" s="1"/>
+      <c r="AK48" s="1"/>
+      <c r="AL48" s="1"/>
+      <c r="AN48" s="1"/>
+      <c r="AO48" s="1"/>
+      <c r="AP48" s="1"/>
+      <c r="AQ48" s="1"/>
+    </row>
+    <row r="49" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+    </row>
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B50" s="10"/>
+      <c r="C50" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
+      <c r="AD50" s="1"/>
+      <c r="AE50" s="1"/>
+      <c r="AF50" s="1"/>
+      <c r="AG50" s="1"/>
+      <c r="AI50" s="1"/>
+      <c r="AJ50" s="1"/>
+      <c r="AK50" s="1"/>
+      <c r="AL50" s="1"/>
+      <c r="AN50" s="1"/>
+      <c r="AO50" s="1"/>
+      <c r="AP50" s="1"/>
+      <c r="AQ50" s="1"/>
+    </row>
+    <row r="51" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+    </row>
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B52" s="10"/>
+      <c r="C52" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="Y52" s="1"/>
+      <c r="Z52" s="1"/>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1"/>
+      <c r="AD52" s="1"/>
+      <c r="AE52" s="1"/>
+      <c r="AF52" s="1"/>
+      <c r="AG52" s="1"/>
+      <c r="AI52" s="1"/>
+      <c r="AJ52" s="1"/>
+      <c r="AK52" s="1"/>
+      <c r="AL52" s="1"/>
+      <c r="AN52" s="1"/>
+      <c r="AO52" s="1"/>
+      <c r="AP52" s="1"/>
+      <c r="AQ52" s="1"/>
+    </row>
+    <row r="53" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+    </row>
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B54" s="10"/>
+      <c r="C54" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="Y54" s="1"/>
+      <c r="Z54" s="1"/>
+      <c r="AA54" s="1"/>
+      <c r="AB54" s="1"/>
+      <c r="AD54" s="1"/>
+      <c r="AE54" s="1"/>
+      <c r="AF54" s="1"/>
+      <c r="AG54" s="1"/>
+      <c r="AI54" s="1"/>
+      <c r="AJ54" s="1"/>
+      <c r="AK54" s="1"/>
+      <c r="AL54" s="1"/>
+      <c r="AN54" s="1"/>
+      <c r="AO54" s="1"/>
+      <c r="AP54" s="1"/>
+      <c r="AQ54" s="1"/>
+    </row>
+    <row r="55" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+    </row>
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B56" s="10"/>
+      <c r="C56" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="Y56" s="1"/>
+      <c r="Z56" s="1"/>
+      <c r="AA56" s="1"/>
+      <c r="AB56" s="1"/>
+      <c r="AD56" s="1"/>
+      <c r="AE56" s="1"/>
+      <c r="AF56" s="1"/>
+      <c r="AG56" s="1"/>
+      <c r="AI56" s="1"/>
+      <c r="AJ56" s="1"/>
+      <c r="AK56" s="1"/>
+      <c r="AL56" s="1"/>
+      <c r="AN56" s="1"/>
+      <c r="AO56" s="1"/>
+      <c r="AP56" s="1"/>
+      <c r="AQ56" s="1"/>
+    </row>
+    <row r="57" spans="1:43" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+    </row>
+    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I58" s="12"/>
+      <c r="J58" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K58" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M58" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="N58" s="12"/>
+      <c r="O58" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="P58" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="R58" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S58" s="12"/>
+      <c r="T58" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="U58" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="V58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="W58" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="X58" s="12"/>
+      <c r="Y58" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z58" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB58" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC58" s="12"/>
+      <c r="AD58" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE58" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG58" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH58" s="12"/>
+      <c r="AI58" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ58" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL58" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM58" s="12"/>
+      <c r="AN58" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO58" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ58" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A59" s="12"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="12"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
+      <c r="M59" s="16"/>
+      <c r="N59" s="12"/>
+      <c r="O59" s="16"/>
+      <c r="P59" s="16"/>
+      <c r="Q59" s="16"/>
+      <c r="R59" s="16"/>
+      <c r="S59" s="12"/>
+      <c r="T59" s="16"/>
+      <c r="U59" s="16"/>
+      <c r="V59" s="16"/>
+      <c r="W59" s="16"/>
+      <c r="X59" s="12"/>
+      <c r="Y59" s="16"/>
+      <c r="Z59" s="16"/>
+      <c r="AA59" s="16"/>
+      <c r="AB59" s="16"/>
+      <c r="AC59" s="12"/>
+      <c r="AD59" s="16"/>
+      <c r="AE59" s="16"/>
+      <c r="AF59" s="16"/>
+      <c r="AG59" s="16"/>
+      <c r="AH59" s="12"/>
+      <c r="AI59" s="16"/>
+      <c r="AJ59" s="16"/>
+      <c r="AK59" s="16"/>
+      <c r="AL59" s="16"/>
+      <c r="AM59" s="12"/>
+      <c r="AN59" s="16"/>
+      <c r="AO59" s="16"/>
+      <c r="AP59" s="16"/>
+      <c r="AQ59" s="16"/>
+    </row>
+    <row r="60" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
+      <c r="O60" s="12"/>
+      <c r="P60" s="12"/>
+      <c r="Q60" s="12"/>
+      <c r="R60" s="12"/>
+      <c r="S60" s="12"/>
+      <c r="T60" s="12"/>
+      <c r="U60" s="12"/>
+      <c r="V60" s="12"/>
+      <c r="W60" s="12"/>
+      <c r="X60" s="12"/>
+      <c r="Y60" s="12"/>
+      <c r="Z60" s="12"/>
+      <c r="AA60" s="12"/>
+      <c r="AB60" s="12"/>
+      <c r="AC60" s="12"/>
+      <c r="AD60" s="12"/>
+      <c r="AE60" s="12"/>
+      <c r="AF60" s="12"/>
+      <c r="AG60" s="12"/>
+      <c r="AH60" s="12"/>
+      <c r="AI60" s="12"/>
+      <c r="AJ60" s="12"/>
+      <c r="AK60" s="12"/>
+      <c r="AL60" s="12"/>
+      <c r="AM60" s="12"/>
+      <c r="AN60" s="12"/>
+      <c r="AO60" s="12"/>
+      <c r="AP60" s="12"/>
+      <c r="AQ60" s="12"/>
+    </row>
+    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A61" s="12"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="12"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="16"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="16"/>
+      <c r="P61" s="16"/>
+      <c r="Q61" s="16"/>
+      <c r="R61" s="16"/>
+      <c r="S61" s="12"/>
+      <c r="T61" s="16"/>
+      <c r="U61" s="16"/>
+      <c r="V61" s="16"/>
+      <c r="W61" s="16"/>
+      <c r="X61" s="12"/>
+      <c r="Y61" s="16"/>
+      <c r="Z61" s="16"/>
+      <c r="AA61" s="16"/>
+      <c r="AB61" s="16"/>
+      <c r="AC61" s="12"/>
+      <c r="AD61" s="16"/>
+      <c r="AE61" s="16"/>
+      <c r="AF61" s="16"/>
+      <c r="AG61" s="16"/>
+      <c r="AH61" s="12"/>
+      <c r="AI61" s="16"/>
+      <c r="AJ61" s="16"/>
+      <c r="AK61" s="16"/>
+      <c r="AL61" s="16"/>
+      <c r="AM61" s="12"/>
+      <c r="AN61" s="16"/>
+      <c r="AO61" s="16"/>
+      <c r="AP61" s="16"/>
+      <c r="AQ61" s="16"/>
+    </row>
+    <row r="62" spans="1:43" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="12"/>
+      <c r="P62" s="12"/>
+      <c r="Q62" s="12"/>
+      <c r="R62" s="12"/>
+      <c r="S62" s="12"/>
+      <c r="T62" s="12"/>
+      <c r="U62" s="12"/>
+      <c r="V62" s="12"/>
+      <c r="W62" s="12"/>
+      <c r="X62" s="12"/>
+      <c r="Y62" s="12"/>
+      <c r="Z62" s="12"/>
+      <c r="AA62" s="12"/>
+      <c r="AB62" s="12"/>
+      <c r="AC62" s="12"/>
+      <c r="AD62" s="12"/>
+      <c r="AE62" s="12"/>
+      <c r="AF62" s="12"/>
+      <c r="AG62" s="12"/>
+      <c r="AH62" s="12"/>
+      <c r="AI62" s="12"/>
+      <c r="AJ62" s="12"/>
+      <c r="AK62" s="12"/>
+      <c r="AL62" s="12"/>
+      <c r="AM62" s="12"/>
+      <c r="AN62" s="12"/>
+      <c r="AO62" s="12"/>
+      <c r="AP62" s="12"/>
+      <c r="AQ62" s="12"/>
+    </row>
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="12"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="16"/>
+      <c r="K63" s="16"/>
+      <c r="L63" s="16"/>
+      <c r="M63" s="16"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="16"/>
+      <c r="P63" s="16"/>
+      <c r="Q63" s="16"/>
+      <c r="R63" s="16"/>
+      <c r="S63" s="12"/>
+      <c r="T63" s="16"/>
+      <c r="U63" s="16"/>
+      <c r="V63" s="16"/>
+      <c r="W63" s="16"/>
+      <c r="X63" s="12"/>
+      <c r="Y63" s="16"/>
+      <c r="Z63" s="16"/>
+      <c r="AA63" s="16"/>
+      <c r="AB63" s="16"/>
+      <c r="AC63" s="12"/>
+      <c r="AD63" s="16"/>
+      <c r="AE63" s="16"/>
+      <c r="AF63" s="16"/>
+      <c r="AG63" s="16"/>
+      <c r="AH63" s="12"/>
+      <c r="AI63" s="16"/>
+      <c r="AJ63" s="16"/>
+      <c r="AK63" s="16"/>
+      <c r="AL63" s="16"/>
+      <c r="AM63" s="12"/>
+      <c r="AN63" s="16"/>
+      <c r="AO63" s="16"/>
+      <c r="AP63" s="16"/>
+      <c r="AQ63" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="AN3:AQ5"/>
+    <mergeCell ref="AN35:AQ37"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="AD3:AG5"/>
+    <mergeCell ref="AD35:AG37"/>
+    <mergeCell ref="AI3:AL5"/>
+    <mergeCell ref="AI35:AL37"/>
+    <mergeCell ref="J3:M5"/>
+    <mergeCell ref="O3:R5"/>
+    <mergeCell ref="T3:W5"/>
+    <mergeCell ref="Y3:AB5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="E35:H37"/>
+    <mergeCell ref="J35:M37"/>
+    <mergeCell ref="O35:R37"/>
+    <mergeCell ref="T35:W37"/>
+    <mergeCell ref="Y35:AB37"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="68" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1962,37 +4560,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
       <c r="N1" s="19"/>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
     </row>
     <row r="3" spans="1:28" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
@@ -2081,32 +4679,32 @@
       <c r="AB5" s="7"/>
     </row>
     <row r="6" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="28"/>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="39"/>
-      <c r="T6" s="37" t="s">
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="51"/>
+      <c r="T6" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="U6" s="38"/>
-      <c r="V6" s="38"/>
-      <c r="W6" s="39"/>
+      <c r="U6" s="50"/>
+      <c r="V6" s="50"/>
+      <c r="W6" s="51"/>
       <c r="X6" s="28"/>
-      <c r="Y6" s="37" t="s">
+      <c r="Y6" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="Z6" s="38"/>
-      <c r="AA6" s="38"/>
-      <c r="AB6" s="39"/>
+      <c r="Z6" s="50"/>
+      <c r="AA6" s="50"/>
+      <c r="AB6" s="51"/>
     </row>
     <row r="7" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
@@ -2723,37 +5321,37 @@
       <c r="R31" s="10"/>
     </row>
     <row r="33" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
       <c r="N33" s="19"/>
-      <c r="P33" s="33" t="s">
+      <c r="P33" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="33"/>
-      <c r="S33" s="33"/>
-      <c r="T33" s="33"/>
-      <c r="U33" s="33"/>
-      <c r="V33" s="33"/>
-      <c r="W33" s="33"/>
-      <c r="X33" s="33"/>
-      <c r="Y33" s="33"/>
-      <c r="Z33" s="33"/>
-      <c r="AA33" s="33"/>
-      <c r="AB33" s="33"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="36"/>
+      <c r="T33" s="36"/>
+      <c r="U33" s="36"/>
+      <c r="V33" s="36"/>
+      <c r="W33" s="36"/>
+      <c r="X33" s="36"/>
+      <c r="Y33" s="36"/>
+      <c r="Z33" s="36"/>
+      <c r="AA33" s="36"/>
+      <c r="AB33" s="36"/>
     </row>
     <row r="35" spans="1:28" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A35" s="29" t="s">
@@ -2842,32 +5440,32 @@
       <c r="AB37" s="7"/>
     </row>
     <row r="38" spans="1:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="E38" s="37" t="s">
+      <c r="E38" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="39"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="51"/>
       <c r="I38" s="28"/>
-      <c r="J38" s="37" t="s">
+      <c r="J38" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="K38" s="38"/>
-      <c r="L38" s="38"/>
-      <c r="M38" s="39"/>
-      <c r="T38" s="37" t="s">
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="51"/>
+      <c r="T38" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="U38" s="38"/>
-      <c r="V38" s="38"/>
-      <c r="W38" s="39"/>
+      <c r="U38" s="50"/>
+      <c r="V38" s="50"/>
+      <c r="W38" s="51"/>
       <c r="X38" s="28"/>
-      <c r="Y38" s="37" t="s">
+      <c r="Y38" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="Z38" s="38"/>
-      <c r="AA38" s="38"/>
-      <c r="AB38" s="39"/>
+      <c r="Z38" s="50"/>
+      <c r="AA38" s="50"/>
+      <c r="AB38" s="51"/>
     </row>
     <row r="39" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="21" t="s">
@@ -3486,14 +6084,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA81F335-DBDD-455C-9B05-7AFC590EC7D7}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AN4" sqref="AN4"/>
     </sheetView>
   </sheetViews>
@@ -3502,38 +6100,38 @@
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="1.7109375" style="45" customWidth="1"/>
+    <col min="4" max="4" width="1.7109375" style="32" customWidth="1"/>
     <col min="5" max="13" width="4" customWidth="1"/>
-    <col min="14" max="14" width="1.7109375" style="45" customWidth="1"/>
+    <col min="14" max="14" width="1.7109375" style="32" customWidth="1"/>
     <col min="15" max="23" width="4" customWidth="1"/>
-    <col min="24" max="24" width="1.7109375" style="45" customWidth="1"/>
+    <col min="24" max="24" width="1.7109375" style="32" customWidth="1"/>
     <col min="25" max="33" width="4" customWidth="1"/>
-    <col min="34" max="34" width="1.7109375" style="45" customWidth="1"/>
+    <col min="34" max="34" width="1.7109375" style="32" customWidth="1"/>
     <col min="35" max="43" width="4" customWidth="1"/>
-    <col min="44" max="44" width="1.7109375" style="45" customWidth="1"/>
+    <col min="44" max="44" width="1.7109375" style="32" customWidth="1"/>
     <col min="45" max="53" width="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AR1" s="44"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AR1" s="31"/>
     </row>
     <row r="2" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
@@ -3558,54 +6156,54 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="10"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="42"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="41"/>
-      <c r="W3" s="42"/>
-      <c r="Y3" s="40"/>
-      <c r="Z3" s="41"/>
-      <c r="AA3" s="41"/>
-      <c r="AB3" s="41"/>
-      <c r="AC3" s="41"/>
-      <c r="AD3" s="41"/>
-      <c r="AE3" s="41"/>
-      <c r="AF3" s="41"/>
-      <c r="AG3" s="42"/>
-      <c r="AI3" s="40"/>
-      <c r="AJ3" s="41"/>
-      <c r="AK3" s="41"/>
-      <c r="AL3" s="41"/>
-      <c r="AM3" s="41"/>
-      <c r="AN3" s="41"/>
-      <c r="AO3" s="41"/>
-      <c r="AP3" s="41"/>
-      <c r="AQ3" s="42"/>
-      <c r="AS3" s="40"/>
-      <c r="AT3" s="41"/>
-      <c r="AU3" s="41"/>
-      <c r="AV3" s="41"/>
-      <c r="AW3" s="41"/>
-      <c r="AX3" s="41"/>
-      <c r="AY3" s="41"/>
-      <c r="AZ3" s="41"/>
-      <c r="BA3" s="42"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="54"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="54"/>
+      <c r="Y3" s="52"/>
+      <c r="Z3" s="53"/>
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="53"/>
+      <c r="AC3" s="53"/>
+      <c r="AD3" s="53"/>
+      <c r="AE3" s="53"/>
+      <c r="AF3" s="53"/>
+      <c r="AG3" s="54"/>
+      <c r="AI3" s="52"/>
+      <c r="AJ3" s="53"/>
+      <c r="AK3" s="53"/>
+      <c r="AL3" s="53"/>
+      <c r="AM3" s="53"/>
+      <c r="AN3" s="53"/>
+      <c r="AO3" s="53"/>
+      <c r="AP3" s="53"/>
+      <c r="AQ3" s="54"/>
+      <c r="AS3" s="52"/>
+      <c r="AT3" s="53"/>
+      <c r="AU3" s="53"/>
+      <c r="AV3" s="53"/>
+      <c r="AW3" s="53"/>
+      <c r="AX3" s="53"/>
+      <c r="AY3" s="53"/>
+      <c r="AZ3" s="53"/>
+      <c r="BA3" s="54"/>
     </row>
     <row r="4" spans="1:53" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="5"/>
@@ -3651,71 +6249,71 @@
       <c r="BA4" s="7"/>
     </row>
     <row r="5" spans="1:53" ht="21" x14ac:dyDescent="0.35">
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="51"/>
       <c r="I5" s="28"/>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="39"/>
-      <c r="O5" s="37" t="s">
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="51"/>
+      <c r="O5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="39"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="51"/>
       <c r="S5" s="28"/>
-      <c r="T5" s="37" t="s">
+      <c r="T5" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="39"/>
-      <c r="Y5" s="37" t="s">
+      <c r="U5" s="50"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="51"/>
+      <c r="Y5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="39"/>
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="50"/>
+      <c r="AB5" s="51"/>
       <c r="AC5" s="28"/>
-      <c r="AD5" s="37" t="s">
+      <c r="AD5" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="AE5" s="38"/>
-      <c r="AF5" s="38"/>
-      <c r="AG5" s="39"/>
-      <c r="AI5" s="37" t="s">
+      <c r="AE5" s="50"/>
+      <c r="AF5" s="50"/>
+      <c r="AG5" s="51"/>
+      <c r="AI5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="AJ5" s="38"/>
-      <c r="AK5" s="38"/>
-      <c r="AL5" s="39"/>
+      <c r="AJ5" s="50"/>
+      <c r="AK5" s="50"/>
+      <c r="AL5" s="51"/>
       <c r="AM5" s="28"/>
-      <c r="AN5" s="37" t="s">
+      <c r="AN5" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="AO5" s="38"/>
-      <c r="AP5" s="38"/>
-      <c r="AQ5" s="39"/>
-      <c r="AS5" s="37" t="s">
+      <c r="AO5" s="50"/>
+      <c r="AP5" s="50"/>
+      <c r="AQ5" s="51"/>
+      <c r="AS5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="AT5" s="38"/>
-      <c r="AU5" s="38"/>
-      <c r="AV5" s="39"/>
+      <c r="AT5" s="50"/>
+      <c r="AU5" s="50"/>
+      <c r="AV5" s="51"/>
       <c r="AW5" s="28"/>
-      <c r="AX5" s="37" t="s">
+      <c r="AX5" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="AY5" s="38"/>
-      <c r="AZ5" s="38"/>
-      <c r="BA5" s="39"/>
+      <c r="AY5" s="50"/>
+      <c r="AZ5" s="50"/>
+      <c r="BA5" s="51"/>
     </row>
     <row r="6" spans="1:53" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -4740,54 +7338,54 @@
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="10"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="42"/>
-      <c r="O30" s="40"/>
-      <c r="P30" s="41"/>
-      <c r="Q30" s="41"/>
-      <c r="R30" s="41"/>
-      <c r="S30" s="41"/>
-      <c r="T30" s="41"/>
-      <c r="U30" s="41"/>
-      <c r="V30" s="41"/>
-      <c r="W30" s="42"/>
-      <c r="Y30" s="40"/>
-      <c r="Z30" s="41"/>
-      <c r="AA30" s="41"/>
-      <c r="AB30" s="41"/>
-      <c r="AC30" s="41"/>
-      <c r="AD30" s="41"/>
-      <c r="AE30" s="41"/>
-      <c r="AF30" s="41"/>
-      <c r="AG30" s="42"/>
-      <c r="AI30" s="40"/>
-      <c r="AJ30" s="41"/>
-      <c r="AK30" s="41"/>
-      <c r="AL30" s="41"/>
-      <c r="AM30" s="41"/>
-      <c r="AN30" s="41"/>
-      <c r="AO30" s="41"/>
-      <c r="AP30" s="41"/>
-      <c r="AQ30" s="42"/>
-      <c r="AS30" s="40"/>
-      <c r="AT30" s="41"/>
-      <c r="AU30" s="41"/>
-      <c r="AV30" s="41"/>
-      <c r="AW30" s="41"/>
-      <c r="AX30" s="41"/>
-      <c r="AY30" s="41"/>
-      <c r="AZ30" s="41"/>
-      <c r="BA30" s="42"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="54"/>
+      <c r="O30" s="52"/>
+      <c r="P30" s="53"/>
+      <c r="Q30" s="53"/>
+      <c r="R30" s="53"/>
+      <c r="S30" s="53"/>
+      <c r="T30" s="53"/>
+      <c r="U30" s="53"/>
+      <c r="V30" s="53"/>
+      <c r="W30" s="54"/>
+      <c r="Y30" s="52"/>
+      <c r="Z30" s="53"/>
+      <c r="AA30" s="53"/>
+      <c r="AB30" s="53"/>
+      <c r="AC30" s="53"/>
+      <c r="AD30" s="53"/>
+      <c r="AE30" s="53"/>
+      <c r="AF30" s="53"/>
+      <c r="AG30" s="54"/>
+      <c r="AI30" s="52"/>
+      <c r="AJ30" s="53"/>
+      <c r="AK30" s="53"/>
+      <c r="AL30" s="53"/>
+      <c r="AM30" s="53"/>
+      <c r="AN30" s="53"/>
+      <c r="AO30" s="53"/>
+      <c r="AP30" s="53"/>
+      <c r="AQ30" s="54"/>
+      <c r="AS30" s="52"/>
+      <c r="AT30" s="53"/>
+      <c r="AU30" s="53"/>
+      <c r="AV30" s="53"/>
+      <c r="AW30" s="53"/>
+      <c r="AX30" s="53"/>
+      <c r="AY30" s="53"/>
+      <c r="AZ30" s="53"/>
+      <c r="BA30" s="54"/>
     </row>
     <row r="31" spans="1:53" ht="21" x14ac:dyDescent="0.35">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B31" s="5"/>
@@ -4833,71 +7431,71 @@
       <c r="BA31" s="7"/>
     </row>
     <row r="32" spans="1:53" ht="21" x14ac:dyDescent="0.35">
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="39"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="51"/>
       <c r="I32" s="28"/>
-      <c r="J32" s="37" t="s">
+      <c r="J32" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="K32" s="38"/>
-      <c r="L32" s="38"/>
-      <c r="M32" s="39"/>
-      <c r="O32" s="37" t="s">
+      <c r="K32" s="50"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="51"/>
+      <c r="O32" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="P32" s="38"/>
-      <c r="Q32" s="38"/>
-      <c r="R32" s="39"/>
+      <c r="P32" s="50"/>
+      <c r="Q32" s="50"/>
+      <c r="R32" s="51"/>
       <c r="S32" s="28"/>
-      <c r="T32" s="37" t="s">
+      <c r="T32" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="U32" s="38"/>
-      <c r="V32" s="38"/>
-      <c r="W32" s="39"/>
-      <c r="Y32" s="37" t="s">
+      <c r="U32" s="50"/>
+      <c r="V32" s="50"/>
+      <c r="W32" s="51"/>
+      <c r="Y32" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="Z32" s="38"/>
-      <c r="AA32" s="38"/>
-      <c r="AB32" s="39"/>
+      <c r="Z32" s="50"/>
+      <c r="AA32" s="50"/>
+      <c r="AB32" s="51"/>
       <c r="AC32" s="28"/>
-      <c r="AD32" s="37" t="s">
+      <c r="AD32" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="AE32" s="38"/>
-      <c r="AF32" s="38"/>
-      <c r="AG32" s="39"/>
-      <c r="AI32" s="37" t="s">
+      <c r="AE32" s="50"/>
+      <c r="AF32" s="50"/>
+      <c r="AG32" s="51"/>
+      <c r="AI32" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="AJ32" s="38"/>
-      <c r="AK32" s="38"/>
-      <c r="AL32" s="39"/>
+      <c r="AJ32" s="50"/>
+      <c r="AK32" s="50"/>
+      <c r="AL32" s="51"/>
       <c r="AM32" s="28"/>
-      <c r="AN32" s="37" t="s">
+      <c r="AN32" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="AO32" s="38"/>
-      <c r="AP32" s="38"/>
-      <c r="AQ32" s="39"/>
-      <c r="AS32" s="37" t="s">
+      <c r="AO32" s="50"/>
+      <c r="AP32" s="50"/>
+      <c r="AQ32" s="51"/>
+      <c r="AS32" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="AT32" s="38"/>
-      <c r="AU32" s="38"/>
-      <c r="AV32" s="39"/>
+      <c r="AT32" s="50"/>
+      <c r="AU32" s="50"/>
+      <c r="AV32" s="51"/>
       <c r="AW32" s="28"/>
-      <c r="AX32" s="37" t="s">
+      <c r="AX32" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="AY32" s="38"/>
-      <c r="AZ32" s="38"/>
-      <c r="BA32" s="39"/>
+      <c r="AY32" s="50"/>
+      <c r="AZ32" s="50"/>
+      <c r="BA32" s="51"/>
     </row>
     <row r="33" spans="1:53" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
@@ -5292,7 +7890,7 @@
       <c r="B39" s="25"/>
       <c r="C39" s="25"/>
     </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:53" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
         <v>32</v>
       </c>
@@ -5897,37 +8495,37 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="E30:M30"/>
-    <mergeCell ref="O30:W30"/>
-    <mergeCell ref="Y30:AG30"/>
-    <mergeCell ref="AI30:AQ30"/>
-    <mergeCell ref="AS30:BA30"/>
     <mergeCell ref="AI3:AQ3"/>
     <mergeCell ref="AI5:AL5"/>
     <mergeCell ref="AN5:AQ5"/>
     <mergeCell ref="AI32:AL32"/>
     <mergeCell ref="AN32:AQ32"/>
+    <mergeCell ref="AI30:AQ30"/>
     <mergeCell ref="AS3:BA3"/>
     <mergeCell ref="AS5:AV5"/>
     <mergeCell ref="AX5:BA5"/>
     <mergeCell ref="AS32:AV32"/>
     <mergeCell ref="AX32:BA32"/>
+    <mergeCell ref="AS30:BA30"/>
     <mergeCell ref="O3:W3"/>
     <mergeCell ref="O5:R5"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="O32:R32"/>
     <mergeCell ref="T32:W32"/>
+    <mergeCell ref="O30:W30"/>
     <mergeCell ref="Y3:AG3"/>
     <mergeCell ref="Y5:AB5"/>
     <mergeCell ref="AD5:AG5"/>
     <mergeCell ref="Y32:AB32"/>
     <mergeCell ref="AD32:AG32"/>
+    <mergeCell ref="Y30:AG30"/>
     <mergeCell ref="E32:H32"/>
     <mergeCell ref="J32:M32"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="E5:H5"/>
     <mergeCell ref="J5:M5"/>
     <mergeCell ref="E3:M3"/>
+    <mergeCell ref="E30:M30"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>